<commit_message>
Replace low ppm resistors
</commit_message>
<xml_diff>
--- a/hardware/pcb/Cape/Project Outputs for Cape/BOM/Bill of Materials-Cape-Prototype.xlsx
+++ b/hardware/pcb/Cape/Project Outputs for Cape/BOM/Bill of Materials-Cape-Prototype.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="719">
   <si>
     <t>Qty</t>
   </si>
@@ -2168,6 +2168,9 @@
   </si>
   <si>
     <t>Total cost</t>
+  </si>
+  <si>
+    <t>ffffffffffffffffffffffffffffff</t>
   </si>
 </sst>
 </file>
@@ -3016,18 +3019,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K62" workbookViewId="0">
-      <selection activeCell="AA87" sqref="AA87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="38" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" customWidth="1"/>
@@ -3419,7 +3422,7 @@
         <v>25</v>
       </c>
       <c r="Y5" t="s">
-        <v>46</v>
+        <v>718</v>
       </c>
       <c r="Z5" t="s">
         <v>34</v>

</xml_diff>